<commit_message>
Actualización y modificación de 3 fracciones del 4to trimestre 2020
</commit_message>
<xml_diff>
--- a/xlsx/a69_f07UPPachuca.xlsx
+++ b/xlsx/a69_f07UPPachuca.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\RH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\SIPOT 4TO TRIMESTRE\Vo.Bo. Uno UPP 4T 2020\4TO TRIMESTRE 2020\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1365,12 +1365,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1654,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,38 +1698,38 @@
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1916,38 +1916,38 @@
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="12"/>
-      <c r="AC6" s="12"/>
-      <c r="AD6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
     </row>
     <row r="7" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2136,10 +2136,10 @@
         <v>2020</v>
       </c>
       <c r="B9" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C9" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>182</v>
@@ -2226,10 +2226,10 @@
         <v>2020</v>
       </c>
       <c r="B10" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C10" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>189</v>
@@ -2316,10 +2316,10 @@
         <v>2020</v>
       </c>
       <c r="B11" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C11" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D11" s="4">
         <v>11</v>
@@ -2406,10 +2406,10 @@
         <v>2020</v>
       </c>
       <c r="B12" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C12" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D12" s="4">
         <v>11</v>
@@ -2496,10 +2496,10 @@
         <v>2020</v>
       </c>
       <c r="B13" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C13" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D13" s="4">
         <v>11</v>
@@ -2586,10 +2586,10 @@
         <v>2020</v>
       </c>
       <c r="B14" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C14" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D14" s="4">
         <v>11</v>
@@ -2676,10 +2676,10 @@
         <v>2020</v>
       </c>
       <c r="B15" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C15" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D15" s="4">
         <v>11</v>
@@ -2766,10 +2766,10 @@
         <v>2020</v>
       </c>
       <c r="B16" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C16" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D16" s="4">
         <v>11</v>
@@ -2856,10 +2856,10 @@
         <v>2020</v>
       </c>
       <c r="B17" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C17" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D17" s="4">
         <v>11</v>
@@ -2946,10 +2946,10 @@
         <v>2020</v>
       </c>
       <c r="B18" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C18" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D18" s="4">
         <v>11</v>
@@ -3036,10 +3036,10 @@
         <v>2020</v>
       </c>
       <c r="B19" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C19" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>231</v>
@@ -3126,10 +3126,10 @@
         <v>2020</v>
       </c>
       <c r="B20" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C20" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>231</v>
@@ -3216,10 +3216,10 @@
         <v>2020</v>
       </c>
       <c r="B21" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C21" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>231</v>
@@ -3306,10 +3306,10 @@
         <v>2020</v>
       </c>
       <c r="B22" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C22" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>231</v>
@@ -3396,10 +3396,10 @@
         <v>2020</v>
       </c>
       <c r="B23" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C23" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>231</v>
@@ -3486,10 +3486,10 @@
         <v>2020</v>
       </c>
       <c r="B24" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C24" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>231</v>
@@ -3576,10 +3576,10 @@
         <v>2020</v>
       </c>
       <c r="B25" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C25" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>231</v>
@@ -3666,10 +3666,10 @@
         <v>2020</v>
       </c>
       <c r="B26" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C26" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>231</v>
@@ -3756,10 +3756,10 @@
         <v>2020</v>
       </c>
       <c r="B27" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C27" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D27" s="4">
         <v>10</v>
@@ -3846,10 +3846,10 @@
         <v>2020</v>
       </c>
       <c r="B28" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C28" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D28" s="4">
         <v>10</v>
@@ -3936,10 +3936,10 @@
         <v>2020</v>
       </c>
       <c r="B29" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C29" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D29" s="4">
         <v>10</v>
@@ -4026,10 +4026,10 @@
         <v>2020</v>
       </c>
       <c r="B30" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C30" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D30" s="4">
         <v>10</v>
@@ -4116,10 +4116,10 @@
         <v>2020</v>
       </c>
       <c r="B31" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C31" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>274</v>
@@ -4206,10 +4206,10 @@
         <v>2020</v>
       </c>
       <c r="B32" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C32" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D32" s="4">
         <v>10</v>
@@ -4296,10 +4296,10 @@
         <v>2020</v>
       </c>
       <c r="B33" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C33" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D33" s="4">
         <v>10</v>
@@ -4388,10 +4388,10 @@
         <v>2020</v>
       </c>
       <c r="B34" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C34" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D34" s="4">
         <v>10</v>
@@ -4478,10 +4478,10 @@
         <v>2020</v>
       </c>
       <c r="B35" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C35" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D35" s="4">
         <v>10</v>
@@ -4568,10 +4568,10 @@
         <v>2020</v>
       </c>
       <c r="B36" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C36" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D36" s="4">
         <v>10</v>
@@ -4658,10 +4658,10 @@
         <v>2020</v>
       </c>
       <c r="B37" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C37" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D37" s="4">
         <v>10</v>
@@ -4748,10 +4748,10 @@
         <v>2020</v>
       </c>
       <c r="B38" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C38" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D38" s="4">
         <v>9</v>
@@ -4838,10 +4838,10 @@
         <v>2020</v>
       </c>
       <c r="B39" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C39" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D39" s="4">
         <v>9</v>
@@ -4928,10 +4928,10 @@
         <v>2020</v>
       </c>
       <c r="B40" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C40" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D40" s="4">
         <v>9</v>
@@ -5018,10 +5018,10 @@
         <v>2020</v>
       </c>
       <c r="B41" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C41" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D41" s="4">
         <v>9</v>
@@ -5108,10 +5108,10 @@
         <v>2020</v>
       </c>
       <c r="B42" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C42" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D42" s="4">
         <v>9</v>
@@ -5198,10 +5198,10 @@
         <v>2020</v>
       </c>
       <c r="B43" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C43" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D43" s="4">
         <v>9</v>
@@ -5288,10 +5288,10 @@
         <v>2020</v>
       </c>
       <c r="B44" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C44" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D44" s="4">
         <v>9</v>
@@ -5378,10 +5378,10 @@
         <v>2020</v>
       </c>
       <c r="B45" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C45" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D45" s="4">
         <v>9</v>
@@ -5468,10 +5468,10 @@
         <v>2020</v>
       </c>
       <c r="B46" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C46" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D46" s="4">
         <v>9</v>
@@ -5558,10 +5558,10 @@
         <v>2020</v>
       </c>
       <c r="B47" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C47" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D47" s="4">
         <v>9</v>
@@ -5648,10 +5648,10 @@
         <v>2020</v>
       </c>
       <c r="B48" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C48" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D48" s="4">
         <v>9</v>
@@ -5738,10 +5738,10 @@
         <v>2020</v>
       </c>
       <c r="B49" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C49" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D49" s="4">
         <v>9</v>
@@ -5828,10 +5828,10 @@
         <v>2020</v>
       </c>
       <c r="B50" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C50" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D50" s="4">
         <v>9</v>
@@ -5918,10 +5918,10 @@
         <v>2020</v>
       </c>
       <c r="B51" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C51" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D51" s="4">
         <v>9</v>
@@ -6008,10 +6008,10 @@
         <v>2020</v>
       </c>
       <c r="B52" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C52" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D52" s="4">
         <v>9</v>
@@ -6098,10 +6098,10 @@
         <v>2020</v>
       </c>
       <c r="B53" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C53" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D53" s="4">
         <v>9</v>
@@ -6188,10 +6188,10 @@
         <v>2020</v>
       </c>
       <c r="B54" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C54" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D54" s="4">
         <v>9</v>
@@ -6278,10 +6278,10 @@
         <v>2020</v>
       </c>
       <c r="B55" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C55" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D55" s="4">
         <v>9</v>
@@ -6366,10 +6366,10 @@
         <v>2020</v>
       </c>
       <c r="B56" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C56" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D56" s="4">
         <v>9</v>
@@ -6456,10 +6456,10 @@
         <v>2020</v>
       </c>
       <c r="B57" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C57" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D57" s="4">
         <v>9</v>
@@ -6546,10 +6546,10 @@
         <v>2020</v>
       </c>
       <c r="B58" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C58" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D58" s="4">
         <v>9</v>
@@ -6636,10 +6636,10 @@
         <v>2020</v>
       </c>
       <c r="B59" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C59" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D59" s="4">
         <v>9</v>
@@ -6726,10 +6726,10 @@
         <v>2020</v>
       </c>
       <c r="B60" s="3">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C60" s="3">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="D60" s="4">
         <v>9</v>
@@ -6904,132 +6904,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="11" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="11" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="11" t="s">
         <v>99</v>
       </c>
     </row>
@@ -7050,207 +7050,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="11" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="11" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="11" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="11" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="11" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="11" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="11" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="11" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="11" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="11" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="11" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="11" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="11" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="11" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="11" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="11" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="11" t="s">
         <v>137</v>
       </c>
     </row>
@@ -7273,162 +7273,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="11" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="11" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="11" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="11" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="11" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="11" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="11" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="11" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="11" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="11" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="11" t="s">
         <v>169</v>
       </c>
     </row>

</xml_diff>